<commit_message>
Common: Some another missing pieces added
</commit_message>
<xml_diff>
--- a/fixtures/atomizers.xlsx
+++ b/fixtures/atomizers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/upgrade/fixtures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFFA0092-E09B-6F40-949F-528D8E9FB50C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89948578-DB0C-44F1-8D82-DA62E01C6716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14520" yWindow="0" windowWidth="14280" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8115" yWindow="1935" windowWidth="40680" windowHeight="18390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="52">
   <si>
     <t>tab</t>
   </si>
@@ -37,9 +37,6 @@
     <t>atomizers</t>
   </si>
   <si>
-    <t>PuffSmith\Atomizer\Import\AtomizerImport</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -94,9 +91,6 @@
     <t>RTA OG 2021</t>
   </si>
   <si>
-    <t>dual</t>
-  </si>
-  <si>
     <t>false</t>
   </si>
   <si>
@@ -133,9 +127,6 @@
     <t>Sirius Mods</t>
   </si>
   <si>
-    <t>Vega RDA </t>
-  </si>
-  <si>
     <t>DL, RDL, MTL</t>
   </si>
   <si>
@@ -148,9 +139,6 @@
     <t>DL, RDL</t>
   </si>
   <si>
-    <t>Hussar Vapes</t>
-  </si>
-  <si>
     <t>Legacy 2 RDA</t>
   </si>
   <si>
@@ -170,6 +158,30 @@
   </si>
   <si>
     <t>MTL, DL, RDL</t>
+  </si>
+  <si>
+    <t>dualCoil</t>
+  </si>
+  <si>
+    <t>atomizer</t>
+  </si>
+  <si>
+    <t>Brunhilde MTL RTA</t>
+  </si>
+  <si>
+    <t>Vapefly</t>
+  </si>
+  <si>
+    <t>MTL RTA 23mm</t>
+  </si>
+  <si>
+    <t>Expromizer V5 MTL RTA</t>
+  </si>
+  <si>
+    <t>Exvape</t>
+  </si>
+  <si>
+    <t>Vega RDA</t>
   </si>
 </sst>
 </file>
@@ -224,11 +236,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Nadpis 2" xfId="1" builtinId="17"/>
@@ -513,16 +524,16 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
     <col min="2" max="2" width="46" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -530,12 +541,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -545,318 +556,379 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{124FA0CC-8DC6-4BC4-980D-0724562E5264}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.5" customWidth="1"/>
-    <col min="2" max="2" width="43.5" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+    <col min="2" max="2" width="43.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="2" t="s">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" t="s">
         <v>28</v>
       </c>
-      <c r="E2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="E16" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>15</v>
       </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" t="s">
-        <v>44</v>
-      </c>
-      <c r="F8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" t="s">
-        <v>46</v>
-      </c>
-      <c r="F9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="B17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" t="s">
         <v>26</v>
       </c>
-      <c r="C11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" t="s">
-        <v>43</v>
-      </c>
-      <c r="F11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" t="s">
-        <v>36</v>
-      </c>
-      <c r="F13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14" t="s">
-        <v>39</v>
-      </c>
-      <c r="F14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="E17" t="s">
         <v>41</v>
       </c>
-      <c r="C15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15" t="s">
-        <v>39</v>
-      </c>
-      <c r="F15" t="s">
-        <v>24</v>
+      <c r="F17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -867,5 +939,6 @@
     <hyperlink ref="A15" r:id="rId4" display="https://www.eliquidshop.cz/vyrobce-hussar-vapes-a1112/" xr:uid="{5D288023-B1E0-C641-AC27-21638FE2A1CC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Common: Prepared very first transaction stuff
</commit_message>
<xml_diff>
--- a/fixtures/atomizers.xlsx
+++ b/fixtures/atomizers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89948578-DB0C-44F1-8D82-DA62E01C6716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B7B48B-3BA6-4D96-BFEE-7759AA6E0974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8115" yWindow="1935" windowWidth="40680" windowHeight="18390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="53">
   <si>
     <t>tab</t>
   </si>
@@ -182,6 +182,9 @@
   </si>
   <si>
     <t>Vega RDA</t>
+  </si>
+  <si>
+    <t>cost</t>
   </si>
 </sst>
 </file>
@@ -556,10 +559,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{124FA0CC-8DC6-4BC4-980D-0724562E5264}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,7 +574,7 @@
     <col min="6" max="6" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -590,8 +593,11 @@
       <c r="F1" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="G1" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -610,8 +616,11 @@
       <c r="F2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -630,8 +639,11 @@
       <c r="F3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -650,8 +662,11 @@
       <c r="F4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -670,8 +685,11 @@
       <c r="F5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -690,8 +708,11 @@
       <c r="F6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -710,8 +731,11 @@
       <c r="F7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -730,8 +754,11 @@
       <c r="F8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -750,8 +777,11 @@
       <c r="F9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -770,8 +800,11 @@
       <c r="F10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -790,8 +823,11 @@
       <c r="F11" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -811,7 +847,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -831,7 +867,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -850,8 +886,11 @@
       <c r="F14" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -870,8 +909,11 @@
       <c r="F15" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -890,8 +932,11 @@
       <c r="F16" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -910,8 +955,11 @@
       <c r="F17" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>50</v>
       </c>

</xml_diff>